<commit_message>
Fix ptp, remove aspen capeg
</commit_message>
<xml_diff>
--- a/application/modules/apps/apppayroll/config/simulasi_pph21.xlsx
+++ b/application/modules/apps/apppayroll/config/simulasi_pph21.xlsx
@@ -9,9 +9,6 @@
   <sheets>
     <sheet name="Gaji Bulan Februari 2018" sheetId="19" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="af">'Gaji Bulan Februari 2018'!$X$4</definedName>
     <definedName name="aw">'Gaji Bulan Februari 2018'!$BN$4</definedName>
@@ -241,9 +238,6 @@
     <t>Nur Ilham</t>
   </si>
   <si>
-    <t>K2</t>
-  </si>
-  <si>
     <t>Menikah</t>
   </si>
   <si>
@@ -251,6 +245,9 @@
   </si>
   <si>
     <t>Astek + Aspe + Askes</t>
+  </si>
+  <si>
+    <t>K3</t>
   </si>
 </sst>
 </file>
@@ -260,7 +257,7 @@
   <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="173" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -524,7 +521,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="12" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -584,16 +581,16 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="2" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="3" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="12" applyFont="1" applyFill="1" applyAlignment="1">
@@ -602,10 +599,10 @@
     <xf numFmtId="41" fontId="2" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="4" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="173" fontId="5" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="11" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -626,6 +623,12 @@
     <xf numFmtId="41" fontId="2" fillId="2" borderId="1" xfId="3" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="12" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -651,12 +654,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="12" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="12" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -702,35 +699,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Education Ekonomi"/>
-      <sheetName val="ASPEN-ASTEK"/>
-      <sheetName val="AnalisisKarir"/>
-      <sheetName val="Education"/>
-      <sheetName val="Pensiun 2012"/>
-      <sheetName val="PerhitunganGajiDir-DP"/>
-      <sheetName val="ResultsGajiBaruNew"/>
-      <sheetName val="Untuk Script"/>
-      <sheetName val="PTKP"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1021,10 +989,10 @@
   <dimension ref="A1:BO36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="AL4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="AC4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D1:D4"/>
+      <selection pane="bottomRight" activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1068,36 +1036,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="45"/>
-      <c r="H1" s="48" t="s">
+      <c r="G1" s="47"/>
+      <c r="H1" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="49"/>
-      <c r="J1" s="48" t="s">
+      <c r="I1" s="51"/>
+      <c r="J1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="49"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="51"/>
       <c r="O1" s="56" t="s">
         <v>30</v>
       </c>
@@ -1161,20 +1129,20 @@
       <c r="BO1" s="13"/>
     </row>
     <row r="2" spans="1:67">
-      <c r="A2" s="55"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="51"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="53"/>
       <c r="O2" s="7" t="s">
         <v>35</v>
       </c>
@@ -1266,13 +1234,13 @@
       <c r="BO2" s="13"/>
     </row>
     <row r="3" spans="1:67">
-      <c r="A3" s="55"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
+      <c r="A3" s="46"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
       <c r="H3" s="1" t="s">
         <v>39</v>
       </c>
@@ -1407,7 +1375,7 @@
         <v>57</v>
       </c>
       <c r="BE3" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BF3" s="37" t="s">
         <v>60</v>
@@ -1437,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>70</v>
@@ -1449,10 +1417,10 @@
         <v>49</v>
       </c>
       <c r="F4" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="40" t="s">
         <v>71</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>72</v>
       </c>
       <c r="H4" s="42">
         <v>1</v>
@@ -1476,25 +1444,27 @@
         <v>0</v>
       </c>
       <c r="O4" s="43">
-        <v>2840885</v>
+        <v>3393916</v>
       </c>
       <c r="P4" s="43">
-        <v>426133</v>
+        <f>O4*15%</f>
+        <v>509087.39999999997</v>
       </c>
       <c r="Q4" s="43">
-        <v>568177</v>
+        <f>O4*10%*3</f>
+        <v>1018174.8</v>
       </c>
       <c r="R4" s="43">
-        <v>400000</v>
+        <v>500000</v>
       </c>
       <c r="S4" s="43">
-        <v>66750</v>
+        <v>82500</v>
       </c>
       <c r="T4" s="43">
-        <v>1500000</v>
+        <v>2250000</v>
       </c>
       <c r="U4" s="43">
-        <v>1592316</v>
+        <v>2202651</v>
       </c>
       <c r="V4" s="44">
         <v>0</v>
@@ -1503,17 +1473,17 @@
         <v>0</v>
       </c>
       <c r="X4" s="43">
-        <v>450000</v>
+        <v>550000</v>
       </c>
       <c r="Y4" s="43">
-        <v>570000</v>
+        <v>660000</v>
       </c>
       <c r="Z4" s="43">
-        <v>800000</v>
+        <v>2370000</v>
       </c>
       <c r="AA4" s="43">
         <f>Y4</f>
-        <v>570000</v>
+        <v>660000</v>
       </c>
       <c r="AB4" s="43">
         <v>0</v>
@@ -1523,36 +1493,36 @@
       </c>
       <c r="AD4" s="44">
         <f ca="1">BL4</f>
-        <v>192592.66666666666</v>
+        <v>867979.66666666663</v>
       </c>
       <c r="AE4" s="44">
         <f ca="1">SUM(O4:AD4)</f>
-        <v>9976853.666666666</v>
+        <v>15064308.866666665</v>
       </c>
       <c r="AF4" s="44">
         <f ca="1">AD4</f>
-        <v>192592.66666666666</v>
+        <v>867979.66666666663</v>
       </c>
       <c r="AG4" s="44">
         <f ca="1">(AE4-Z4)*2%</f>
-        <v>183537.07333333333</v>
+        <v>253886.17733333333</v>
       </c>
       <c r="AH4" s="44">
         <v>47250</v>
       </c>
       <c r="AI4" s="44">
         <f>(SUM(O4:Q4)+X4)*5%</f>
-        <v>214259.75</v>
+        <v>273558.91000000003</v>
       </c>
       <c r="AJ4" s="44">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="AK4" s="44"/>
       <c r="AL4" s="44">
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="AM4" s="44">
-        <v>206000</v>
+        <v>0</v>
       </c>
       <c r="AN4" s="44">
         <v>0</v>
@@ -1561,19 +1531,18 @@
         <v>0</v>
       </c>
       <c r="AP4" s="44">
-        <f ca="1">2.5%*AE4</f>
-        <v>249421.34166666667</v>
+        <v>376608</v>
       </c>
       <c r="AQ4" s="44">
         <v>0</v>
       </c>
       <c r="AR4" s="43">
         <f ca="1">SUM(AF4:AQ4)</f>
-        <v>1193060.8316666665</v>
+        <v>1829282.7540000002</v>
       </c>
       <c r="AS4" s="43">
         <f ca="1">AE4-AR4</f>
-        <v>8783792.834999999</v>
+        <v>13235026.112666665</v>
       </c>
       <c r="AT4" s="31"/>
       <c r="AU4" s="11"/>
@@ -1584,15 +1553,15 @@
       <c r="AX4" s="11"/>
       <c r="AY4" s="33">
         <f ca="1">AE4</f>
-        <v>9976853.666666666</v>
+        <v>15064308.866666665</v>
       </c>
       <c r="AZ4" s="33">
         <f ca="1">AG4</f>
-        <v>183537.07333333333</v>
+        <v>253886.17733333333</v>
       </c>
       <c r="BA4" s="33">
         <f>AI4</f>
-        <v>214259.75</v>
+        <v>273558.91000000003</v>
       </c>
       <c r="BB4" s="33">
         <f>AH4</f>
@@ -1600,7 +1569,7 @@
       </c>
       <c r="BC4" s="33">
         <f ca="1">SUM(AY4:BB4)</f>
-        <v>10421900.49</v>
+        <v>15639003.953999998</v>
       </c>
       <c r="BD4" s="33">
         <f ca="1">IF((5%*BC4)&lt;=500000,BC4*5%,500000)</f>
@@ -1608,39 +1577,39 @@
       </c>
       <c r="BE4" s="33">
         <f ca="1">SUM(AZ4:BB4)</f>
-        <v>445046.82333333336</v>
+        <v>574695.08733333333</v>
       </c>
       <c r="BF4" s="33">
         <f ca="1">SUM(BD4:BE4)</f>
-        <v>945046.82333333336</v>
+        <v>1074695.0873333332</v>
       </c>
       <c r="BG4" s="33">
         <f ca="1">BC4-BF4</f>
-        <v>9476853.666666666</v>
+        <v>14564308.866666665</v>
       </c>
       <c r="BH4" s="33">
         <f ca="1">BG4*12</f>
-        <v>113722244</v>
+        <v>174771706.39999998</v>
       </c>
       <c r="BI4" s="33">
-        <v>67500000</v>
+        <v>72000000</v>
       </c>
       <c r="BJ4" s="33">
         <f ca="1">IF(BH4-BI4&gt;0,BH4-BI4,0)</f>
-        <v>46222244</v>
+        <v>102771706.39999998</v>
       </c>
       <c r="BK4" s="34">
         <f ca="1">ROUND(IF(BJ4&lt;=0,0,IF(BJ4&lt;=50000000,(BJ4*5%),IF(BJ4&gt;500000000,((BJ4-500000000)*30%)+95000000,IF(BJ4&gt;250000000,((BJ4-250000000)*25%)+32500000,IF(BJ4&gt;50000000,(((BJ4-50000000)*15%)+2500000)))))),0)</f>
-        <v>2311112</v>
+        <v>10415756</v>
       </c>
       <c r="BL4" s="33">
         <f ca="1">BK4/12</f>
-        <v>192592.66666666666</v>
+        <v>867979.66666666663</v>
       </c>
       <c r="BM4" s="11"/>
       <c r="BN4" s="11">
         <f ca="1">AS4-AW4</f>
-        <v>8783792.834999999</v>
+        <v>13235026.112666665</v>
       </c>
       <c r="BO4" s="13"/>
     </row>
@@ -1744,7 +1713,10 @@
       <c r="AB6" s="17"/>
       <c r="AC6" s="17"/>
       <c r="AD6" s="18"/>
-      <c r="AE6" s="18"/>
+      <c r="AE6" s="18">
+        <f ca="1">AE4-AD4</f>
+        <v>14196329.199999999</v>
+      </c>
       <c r="AF6" s="18"/>
       <c r="AG6" s="18"/>
       <c r="AH6" s="18"/>
@@ -1813,7 +1785,10 @@
       <c r="AB7" s="17"/>
       <c r="AC7" s="17"/>
       <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
+      <c r="AE7" s="18">
+        <f ca="1">AE6*2.5</f>
+        <v>35490823</v>
+      </c>
       <c r="AF7" s="18"/>
       <c r="AG7" s="18"/>
       <c r="AH7" s="18"/>
@@ -1882,7 +1857,9 @@
       <c r="AB8" s="17"/>
       <c r="AC8" s="17"/>
       <c r="AD8" s="18"/>
-      <c r="AE8" s="18"/>
+      <c r="AE8" s="18">
+        <v>36129760</v>
+      </c>
       <c r="AF8" s="18"/>
       <c r="AG8" s="18"/>
       <c r="AH8" s="18"/>
@@ -1952,7 +1929,10 @@
       <c r="AC9" s="17"/>
       <c r="AD9" s="18"/>
       <c r="AE9" s="18"/>
-      <c r="AF9" s="18"/>
+      <c r="AF9" s="18">
+        <f>AE8/2.5</f>
+        <v>14451904</v>
+      </c>
       <c r="AG9" s="18"/>
       <c r="AH9" s="18"/>
       <c r="AI9" s="18"/>
@@ -3749,21 +3729,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="O1:AD1"/>
     <mergeCell ref="AS1:AS3"/>
     <mergeCell ref="P2:AD2"/>
     <mergeCell ref="AE1:AE3"/>
     <mergeCell ref="AF1:AR1"/>
     <mergeCell ref="AF2:AQ2"/>
-    <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
     <mergeCell ref="H1:I2"/>
     <mergeCell ref="J1:N2"/>
+    <mergeCell ref="O1:AD1"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:E3"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>